<commit_message>
✨ feat(zonal_statistics cli and 111):
</commit_message>
<xml_diff>
--- a/config/cfg_template.xlsx
+++ b/config/cfg_template.xlsx
@@ -4,18 +4,19 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="26880" windowHeight="10560"/>
+    <workbookView windowWidth="25600" windowHeight="9560" activeTab="1"/>
   </bookViews>
   <sheets>
     <sheet name="JSBG_7_PH-(表层样点土壤PH分级统计表)" sheetId="1" r:id="rId1"/>
-    <sheet name="JSBG_7_SOM-(表层样点土壤SOM分级统计表)" sheetId="2" r:id="rId2"/>
+    <sheet name="JSBG_8_OM-(表层样点土壤OM分级统计表)" sheetId="2" r:id="rId2"/>
+    <sheet name="TRSX_111_PH-(土地利用类型土壤pH分级面积统计表" sheetId="3" r:id="rId3"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="32" uniqueCount="22">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
   <si>
     <t>A1</t>
   </si>
@@ -41,6 +42,27 @@
     <t>级别范围</t>
   </si>
   <si>
+    <t>B3</t>
+  </si>
+  <si>
+    <t>均值</t>
+  </si>
+  <si>
+    <t>计数（个）</t>
+  </si>
+  <si>
+    <t>占比</t>
+  </si>
+  <si>
+    <t>SOM分级</t>
+  </si>
+  <si>
+    <t>XX县土地利用类型土壤pH分级面积统计表</t>
+  </si>
+  <si>
+    <t>土地利用类型</t>
+  </si>
+  <si>
     <t>6.5-7.5</t>
   </si>
   <si>
@@ -56,31 +78,19 @@
     <t>&gt;8.5, ≤4.5</t>
   </si>
   <si>
-    <t>均值</t>
-  </si>
-  <si>
-    <t>计数（个）</t>
-  </si>
-  <si>
-    <t>占比</t>
-  </si>
-  <si>
-    <t>SOM分级</t>
-  </si>
-  <si>
-    <t>&gt;35.00</t>
-  </si>
-  <si>
-    <t>25.00-35.00</t>
-  </si>
-  <si>
-    <t>15.00-25.00</t>
-  </si>
-  <si>
-    <t>10.00-15.00</t>
-  </si>
-  <si>
-    <t>≤10.00</t>
+    <t>耕地</t>
+  </si>
+  <si>
+    <t>园地</t>
+  </si>
+  <si>
+    <t>林地</t>
+  </si>
+  <si>
+    <t>草地</t>
+  </si>
+  <si>
+    <t>合计</t>
   </si>
 </sst>
 </file>
@@ -109,18 +119,18 @@
       <charset val="134"/>
     </font>
     <font>
-      <sz val="11"/>
-      <color theme="1"/>
-      <name val="微软雅黑"/>
-      <charset val="134"/>
-    </font>
-    <font>
       <sz val="10"/>
       <color rgb="FF000000"/>
       <name val="微软雅黑"/>
       <charset val="134"/>
     </font>
     <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="微软雅黑"/>
+      <charset val="134"/>
+    </font>
+    <font>
       <u/>
       <sz val="11"/>
       <color rgb="FF0000FF"/>
@@ -465,7 +475,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="10">
+  <borders count="12">
     <border>
       <left/>
       <right/>
@@ -483,6 +493,32 @@
       <top style="thin">
         <color auto="1"/>
       </top>
+      <bottom style="thin">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top style="thin">
+        <color auto="1"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
       <bottom style="thin">
         <color auto="1"/>
       </bottom>
@@ -612,7 +648,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="2" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -624,34 +660,34 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="3" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="11" fillId="0" borderId="4" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="11" fillId="0" borderId="6" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="6" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="5" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="16" fillId="0" borderId="8" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="17" fillId="0" borderId="9" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="15" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -736,27 +772,36 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="49">
@@ -1285,8 +1330,8 @@
   <sheetPr/>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F11" sqref="F11"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B3" sqref="B3:F6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="5"/>
@@ -1307,7 +1352,7 @@
       <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="7" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1327,99 +1372,55 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="2" t="s">
+      <c r="A3" s="7" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
         <v>8</v>
       </c>
-      <c r="C3" s="3" t="s">
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="8" t="s">
         <v>9</v>
       </c>
-      <c r="D3" s="3" t="s">
-        <v>10</v>
-      </c>
-      <c r="E3" s="3" t="s">
-        <v>11</v>
-      </c>
-      <c r="F3" s="3" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="5" t="str">
+      <c r="B4" s="9" t="str">
         <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
         <v>B4</v>
       </c>
-      <c r="C4" s="5" t="str">
-        <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
-        <v>C4</v>
-      </c>
-      <c r="D4" s="5" t="str">
-        <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
-        <v>D4</v>
-      </c>
-      <c r="E4" s="5" t="str">
-        <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
-        <v>E4</v>
-      </c>
-      <c r="F4" s="5" t="str">
-        <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
-        <v>F4</v>
-      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="5" t="str">
+      <c r="A5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="9" t="str">
         <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
         <v>B5</v>
       </c>
-      <c r="C5" s="5" t="str">
-        <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
-        <v>C5</v>
-      </c>
-      <c r="D5" s="5" t="str">
-        <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
-        <v>D5</v>
-      </c>
-      <c r="E5" s="5" t="str">
-        <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
-        <v>E5</v>
-      </c>
-      <c r="F5" s="5" t="str">
-        <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
-        <v>F5</v>
-      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="5" t="str">
+      <c r="A6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="9" t="str">
         <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
         <v>B6</v>
       </c>
-      <c r="C6" s="5" t="str">
-        <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
-        <v>C6</v>
-      </c>
-      <c r="D6" s="5" t="str">
-        <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
-        <v>D6</v>
-      </c>
-      <c r="E6" s="5" t="str">
-        <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
-        <v>E6</v>
-      </c>
-      <c r="F6" s="5" t="str">
-        <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
-        <v>F6</v>
-      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1435,8 +1436,8 @@
   <sheetPr/>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="H9" sqref="H9"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="5"/>
@@ -1448,18 +1449,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="1" t="s">
+      <c r="A1" s="6" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="1"/>
-      <c r="C1" s="1"/>
-      <c r="D1" s="1"/>
-      <c r="E1" s="1"/>
-      <c r="F1" s="1"/>
+      <c r="B1" s="6"/>
+      <c r="C1" s="6"/>
+      <c r="D1" s="6"/>
+      <c r="E1" s="6"/>
+      <c r="F1" s="6"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
-        <v>16</v>
+      <c r="A2" s="7" t="s">
+        <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
         <v>2</v>
@@ -1478,99 +1479,55 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="4" t="s">
+      <c r="A3" s="8" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="4" t="s">
-        <v>17</v>
-      </c>
-      <c r="C3" s="4" t="s">
-        <v>18</v>
-      </c>
-      <c r="D3" s="4" t="s">
-        <v>19</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>20</v>
-      </c>
-      <c r="F3" s="4" t="s">
-        <v>21</v>
-      </c>
+      <c r="B3" s="3" t="s">
+        <v>8</v>
+      </c>
+      <c r="C3" s="3"/>
+      <c r="D3" s="3"/>
+      <c r="E3" s="3"/>
+      <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="4" t="s">
-        <v>13</v>
-      </c>
-      <c r="B4" s="5" t="str">
-        <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
+      <c r="A4" s="8" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="9" t="str">
+        <f t="shared" ref="B4:B6" si="0">SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
         <v>B4</v>
       </c>
-      <c r="C4" s="5" t="str">
-        <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
-        <v>C4</v>
-      </c>
-      <c r="D4" s="5" t="str">
-        <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
-        <v>D4</v>
-      </c>
-      <c r="E4" s="5" t="str">
-        <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
-        <v>E4</v>
-      </c>
-      <c r="F4" s="5" t="str">
-        <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
-        <v>F4</v>
-      </c>
+      <c r="C4" s="9"/>
+      <c r="D4" s="9"/>
+      <c r="E4" s="9"/>
+      <c r="F4" s="9"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="4" t="s">
-        <v>14</v>
-      </c>
-      <c r="B5" s="5" t="str">
-        <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
+      <c r="A5" s="8" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="9" t="str">
+        <f t="shared" si="0"/>
         <v>B5</v>
       </c>
-      <c r="C5" s="5" t="str">
-        <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
-        <v>C5</v>
-      </c>
-      <c r="D5" s="5" t="str">
-        <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
-        <v>D5</v>
-      </c>
-      <c r="E5" s="5" t="str">
-        <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
-        <v>E5</v>
-      </c>
-      <c r="F5" s="5" t="str">
-        <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
-        <v>F5</v>
-      </c>
+      <c r="C5" s="9"/>
+      <c r="D5" s="9"/>
+      <c r="E5" s="9"/>
+      <c r="F5" s="9"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="4" t="s">
-        <v>15</v>
-      </c>
-      <c r="B6" s="5" t="str">
-        <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
+      <c r="A6" s="8" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="9" t="str">
+        <f t="shared" si="0"/>
         <v>B6</v>
       </c>
-      <c r="C6" s="5" t="str">
-        <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
-        <v>C6</v>
-      </c>
-      <c r="D6" s="5" t="str">
-        <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
-        <v>D6</v>
-      </c>
-      <c r="E6" s="5" t="str">
-        <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
-        <v>E6</v>
-      </c>
-      <c r="F6" s="5" t="str">
-        <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
-        <v>F6</v>
-      </c>
+      <c r="C6" s="9"/>
+      <c r="D6" s="9"/>
+      <c r="E6" s="9"/>
+      <c r="F6" s="9"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1579,4 +1536,128 @@
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I2" sqref="I2"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="7" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="13.6153846153846" customWidth="1"/>
+    <col min="2" max="5" width="8.07692307692308" customWidth="1"/>
+    <col min="6" max="6" width="11.2307692307692" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>13</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>14</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="4"/>
+      <c r="B3" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="5" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="5" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="5" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="5" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="5" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
✨ feat(finish 7 10 16 19 22 25 28 31 34 37 40 43 46 49 53):
</commit_message>
<xml_diff>
--- a/config/cfg_template.xlsx
+++ b/config/cfg_template.xlsx
@@ -4,19 +4,32 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="9560" activeTab="1"/>
+    <workbookView windowWidth="25600" windowHeight="9560" firstSheet="14" activeTab="14"/>
   </bookViews>
   <sheets>
-    <sheet name="JSBG_7_PH-(表层样点土壤PH分级统计表)" sheetId="1" r:id="rId1"/>
-    <sheet name="JSBG_8_OM-(表层样点土壤OM分级统计表)" sheetId="2" r:id="rId2"/>
-    <sheet name="TRSX_111_PH-(土地利用类型土壤pH分级面积统计表" sheetId="3" r:id="rId3"/>
+    <sheet name="JSBG_7_PH-(表层样PH分级)" sheetId="1" r:id="rId1"/>
+    <sheet name="JSBG_10_OM-(表层样OM分级)" sheetId="2" r:id="rId2"/>
+    <sheet name="JSBG_16_TN-(表层样TN分级)" sheetId="5" r:id="rId3"/>
+    <sheet name="JSBG_19_TP-(表层样TP分级)" sheetId="6" r:id="rId4"/>
+    <sheet name="JSBG_22_TK-(表层样TK分级)" sheetId="7" r:id="rId5"/>
+    <sheet name="JSBG_25_AP-(表层样AP分级)" sheetId="8" r:id="rId6"/>
+    <sheet name="JSBG_28_AK-(表层样AK分级)" sheetId="9" r:id="rId7"/>
+    <sheet name="JSBG_31_AS1-(表层样AS1分级)" sheetId="10" r:id="rId8"/>
+    <sheet name="JSBG_34_AFE-(表层样AFE分级)" sheetId="11" r:id="rId9"/>
+    <sheet name="JSBG_37_AMN-(表层样AMN分级)" sheetId="12" r:id="rId10"/>
+    <sheet name="JSBG_40_ACU-(表层样ACU分级)" sheetId="13" r:id="rId11"/>
+    <sheet name="JSBG_43_AZN-(表层样AZN分级)" sheetId="14" r:id="rId12"/>
+    <sheet name="JSBG_46_AB-(表层样AB分级)" sheetId="4" r:id="rId13"/>
+    <sheet name="JSBG_49_AMO-(表层样AMO分级)" sheetId="15" r:id="rId14"/>
+    <sheet name="JSBG_53_GZCHD-(表层样GZCHD分级)" sheetId="16" r:id="rId15"/>
+    <sheet name="TRSX_111_PH-(利用类型pH面积分级)" sheetId="3" r:id="rId16"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="41" uniqueCount="25">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="249" uniqueCount="108">
   <si>
     <t>A1</t>
   </si>
@@ -55,6 +68,255 @@
   </si>
   <si>
     <t>SOM分级</t>
+  </si>
+  <si>
+    <t>XX县表层样点土壤全氮含量分级统计表</t>
+  </si>
+  <si>
+    <t>TN分级</t>
+  </si>
+  <si>
+    <t>&gt;2.00</t>
+  </si>
+  <si>
+    <t>1.50-2.00</t>
+  </si>
+  <si>
+    <t>1.00-1.50</t>
+  </si>
+  <si>
+    <t>0.75-1.00</t>
+  </si>
+  <si>
+    <t>≤0.75</t>
+  </si>
+  <si>
+    <t>XX县表层样点土壤全磷含量分级统计表</t>
+  </si>
+  <si>
+    <t>TP分级</t>
+  </si>
+  <si>
+    <t>&gt;1.00</t>
+  </si>
+  <si>
+    <t>0.80-1.00</t>
+  </si>
+  <si>
+    <t>0.60-0.80</t>
+  </si>
+  <si>
+    <t>0.40-0.60</t>
+  </si>
+  <si>
+    <t>≤0.40</t>
+  </si>
+  <si>
+    <t>XX县表层样点土壤全钾含量分级统计表</t>
+  </si>
+  <si>
+    <t>TK分级</t>
+  </si>
+  <si>
+    <t>&gt;25.00</t>
+  </si>
+  <si>
+    <t>20.00-25.00</t>
+  </si>
+  <si>
+    <t>15.00-20.00</t>
+  </si>
+  <si>
+    <t>10.00-15.00</t>
+  </si>
+  <si>
+    <t>≤10.00</t>
+  </si>
+  <si>
+    <t>XX县表层样点土壤有效磷含量分级统计表</t>
+  </si>
+  <si>
+    <t>AP分级</t>
+  </si>
+  <si>
+    <t>&gt;35.00</t>
+  </si>
+  <si>
+    <t>25.00-35.00</t>
+  </si>
+  <si>
+    <t>15.00-25.00</t>
+  </si>
+  <si>
+    <t>XX县表层样点土壤速效钾含量分级统计表</t>
+  </si>
+  <si>
+    <t>AK分级</t>
+  </si>
+  <si>
+    <t>&gt;150</t>
+  </si>
+  <si>
+    <t>125~150</t>
+  </si>
+  <si>
+    <t>100~125</t>
+  </si>
+  <si>
+    <t>75~100</t>
+  </si>
+  <si>
+    <t>≤75</t>
+  </si>
+  <si>
+    <t>XX县表层样点土壤有效硫含量分级统计表</t>
+  </si>
+  <si>
+    <t>有效硫分级</t>
+  </si>
+  <si>
+    <t>&gt;40.00</t>
+  </si>
+  <si>
+    <t>30.00-40.00</t>
+  </si>
+  <si>
+    <t>20.00-30.00</t>
+  </si>
+  <si>
+    <t>10.00-20.00</t>
+  </si>
+  <si>
+    <t>XX县表层样点土壤有效铁含量分级统计表</t>
+  </si>
+  <si>
+    <t>有效铁分级</t>
+  </si>
+  <si>
+    <t>&gt;20.00</t>
+  </si>
+  <si>
+    <t>4.50-10.00</t>
+  </si>
+  <si>
+    <t>2.50-4.50</t>
+  </si>
+  <si>
+    <t>≤2.50</t>
+  </si>
+  <si>
+    <t>XX县表层样点土壤有效锰含量分级统计表</t>
+  </si>
+  <si>
+    <t>有效锰分级</t>
+  </si>
+  <si>
+    <t>&gt;50.00</t>
+  </si>
+  <si>
+    <t>15.00-50.00</t>
+  </si>
+  <si>
+    <t>7.00-15.00</t>
+  </si>
+  <si>
+    <t>3.00-7.00</t>
+  </si>
+  <si>
+    <t>≤3.00</t>
+  </si>
+  <si>
+    <t>XX县表层样点土壤有效铜含量分级统计表</t>
+  </si>
+  <si>
+    <t>有效铜分级</t>
+  </si>
+  <si>
+    <t>&gt;1.80</t>
+  </si>
+  <si>
+    <t>1.00-1.80</t>
+  </si>
+  <si>
+    <t>0.20-1.00</t>
+  </si>
+  <si>
+    <t>0.10-0.20</t>
+  </si>
+  <si>
+    <t>≤0.10</t>
+  </si>
+  <si>
+    <t>XX县表层样点土壤有效锌含量分级统计表</t>
+  </si>
+  <si>
+    <t>有效锌分级</t>
+  </si>
+  <si>
+    <t>&gt;3.00</t>
+  </si>
+  <si>
+    <t>2.00-3.00</t>
+  </si>
+  <si>
+    <t>1.00-2.00</t>
+  </si>
+  <si>
+    <t>0.50-1.00</t>
+  </si>
+  <si>
+    <t>≤0.50</t>
+  </si>
+  <si>
+    <t>XX县表层样点土壤有效硼含量分级统计表</t>
+  </si>
+  <si>
+    <t>有效硼分级</t>
+  </si>
+  <si>
+    <t>0.25-0.50</t>
+  </si>
+  <si>
+    <t>≤0.25</t>
+  </si>
+  <si>
+    <t>XX县表层样点土壤有效钼含量分级统计表</t>
+  </si>
+  <si>
+    <t>有效钼分级</t>
+  </si>
+  <si>
+    <t>&gt;0.20</t>
+  </si>
+  <si>
+    <t>0.15-0.20</t>
+  </si>
+  <si>
+    <t>0.10-0.15</t>
+  </si>
+  <si>
+    <t>0.05-0.10</t>
+  </si>
+  <si>
+    <t>≤0.05</t>
+  </si>
+  <si>
+    <t>XX县表层样点耕层厚度分级统计表</t>
+  </si>
+  <si>
+    <t>耕层厚度分级</t>
+  </si>
+  <si>
+    <t>16.00-20.00</t>
+  </si>
+  <si>
+    <t>12.00-16.00</t>
+  </si>
+  <si>
+    <t>8.00-12.00</t>
+  </si>
+  <si>
+    <t>≤8.00</t>
   </si>
   <si>
     <t>XX县土地利用类型土壤pH分级面积统计表</t>
@@ -772,7 +1034,7 @@
       <alignment vertical="center"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="12">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -791,10 +1053,16 @@
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="10" fontId="3" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="3" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
@@ -1342,17 +1610,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1372,7 +1640,7 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="7" t="s">
+      <c r="A3" s="6" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1384,47 +1652,771 @@
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="9" t="str">
+      <c r="B4" s="11" t="str">
         <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
         <v>B4</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="9" t="str">
+      <c r="B5" s="11" t="str">
         <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
         <v>B5</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="9" t="str">
+      <c r="B6" s="11" t="str">
         <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
         <v>B6</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>58</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="6" t="s">
+        <v>59</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>60</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>61</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>62</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>63</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>64</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>65</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="6" t="s">
+        <v>66</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>69</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>70</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>71</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet12.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>72</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>74</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>75</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>78</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet13.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F3" sqref="F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>79</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="6" t="s">
+        <v>80</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>76</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>77</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>81</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="7"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet14.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>83</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="6" t="s">
+        <v>84</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>85</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>86</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>87</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>88</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>89</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet15.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J8" sqref="J8"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>90</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="6" t="s">
+        <v>91</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>92</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>93</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>94</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet16.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M19" sqref="M19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="7" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="13.6153846153846" customWidth="1"/>
+    <col min="2" max="5" width="8.07692307692308" customWidth="1"/>
+    <col min="6" max="6" width="11.2307692307692" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>96</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="4"/>
+      <c r="B3" s="3" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="3" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="3" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>102</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="5" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="5"/>
+      <c r="C4" s="5"/>
+      <c r="D4" s="5"/>
+      <c r="E4" s="5"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="5" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="5"/>
+      <c r="C5" s="5"/>
+      <c r="D5" s="5"/>
+      <c r="E5" s="5"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="5" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="5"/>
+      <c r="C6" s="5"/>
+      <c r="D6" s="5"/>
+      <c r="E6" s="5"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="5" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="5"/>
+      <c r="C7" s="5"/>
+      <c r="D7" s="5"/>
+      <c r="E7" s="5"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="5" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -1436,8 +2428,8 @@
   <sheetPr/>
   <dimension ref="A1:F6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="5"/>
@@ -1449,17 +2441,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="6" t="s">
+      <c r="A1" s="9" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="6"/>
-      <c r="C1" s="6"/>
-      <c r="D1" s="6"/>
-      <c r="E1" s="6"/>
-      <c r="F1" s="6"/>
+      <c r="B1" s="9"/>
+      <c r="C1" s="9"/>
+      <c r="D1" s="9"/>
+      <c r="E1" s="9"/>
+      <c r="F1" s="9"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="7" t="s">
+      <c r="A2" s="6" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1479,7 +2471,7 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="3" t="s">
@@ -1491,43 +2483,43 @@
       <c r="F3" s="3"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="8" t="s">
+      <c r="A4" s="10" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="9" t="str">
+      <c r="B4" s="11" t="str">
         <f t="shared" ref="B4:B6" si="0">SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
         <v>B4</v>
       </c>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="8" t="s">
+      <c r="A5" s="10" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="9" t="str">
+      <c r="B5" s="11" t="str">
         <f t="shared" si="0"/>
         <v>B5</v>
       </c>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="8" t="s">
+      <c r="A6" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="9" t="str">
+      <c r="B6" s="11" t="str">
         <f t="shared" si="0"/>
         <v>B6</v>
       </c>
-      <c r="C6" s="9"/>
-      <c r="D6" s="9"/>
-      <c r="E6" s="9"/>
-      <c r="F6" s="9"/>
+      <c r="C6" s="11"/>
+      <c r="D6" s="11"/>
+      <c r="E6" s="11"/>
+      <c r="F6" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1541,18 +2533,13 @@
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I2" sqref="I2"/>
+      <selection activeCell="A1" sqref="A1:F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="7" outlineLevelCol="5"/>
-  <cols>
-    <col min="1" max="1" width="13.6153846153846" customWidth="1"/>
-    <col min="2" max="5" width="8.07692307692308" customWidth="1"/>
-    <col min="6" max="6" width="11.2307692307692" customWidth="1"/>
-  </cols>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="5"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
@@ -1565,7 +2552,7 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="2" t="s">
+      <c r="A2" s="6" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="3" t="s">
@@ -1585,77 +2572,658 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="4"/>
+      <c r="A3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>15</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>20</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="6" t="s">
+        <v>21</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>26</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>27</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="6" t="s">
+        <v>28</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>30</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>31</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>34</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="6" t="s">
+        <v>35</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>37</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>38</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>32</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>39</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="6" t="s">
+        <v>40</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="7" t="s">
+        <v>7</v>
+      </c>
       <c r="B3" s="3" t="s">
-        <v>15</v>
+        <v>41</v>
       </c>
       <c r="C3" s="3" t="s">
-        <v>16</v>
+        <v>42</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="E3" s="3" t="s">
-        <v>18</v>
+        <v>44</v>
       </c>
       <c r="F3" s="3" t="s">
-        <v>19</v>
+        <v>45</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="5" t="s">
-        <v>20</v>
-      </c>
-      <c r="B4" s="5"/>
-      <c r="C4" s="5"/>
-      <c r="D4" s="5"/>
-      <c r="E4" s="5"/>
-      <c r="F4" s="5"/>
+      <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="5" t="s">
-        <v>21</v>
-      </c>
-      <c r="B5" s="5"/>
-      <c r="C5" s="5"/>
-      <c r="D5" s="5"/>
-      <c r="E5" s="5"/>
-      <c r="F5" s="5"/>
+      <c r="A5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="5" t="s">
-        <v>22</v>
-      </c>
-      <c r="B6" s="5"/>
-      <c r="C6" s="5"/>
-      <c r="D6" s="5"/>
-      <c r="E6" s="5"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="5" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="5"/>
-      <c r="C7" s="5"/>
-      <c r="D7" s="5"/>
-      <c r="E7" s="5"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="5" t="s">
-        <v>24</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="A6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
     </row>
   </sheetData>
-  <mergeCells count="2">
+  <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
-    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>46</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="6" t="s">
+        <v>47</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>48</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>49</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>50</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="8"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F6"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F6"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="5" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>52</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="6" t="s">
+        <v>53</v>
+      </c>
+      <c r="B2" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="3" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="3" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="3" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="7" t="s">
+        <v>7</v>
+      </c>
+      <c r="B3" s="7" t="s">
+        <v>54</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>51</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>55</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>56</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="7" t="s">
+        <v>9</v>
+      </c>
+      <c r="B4" s="7"/>
+      <c r="C4" s="7"/>
+      <c r="D4" s="7"/>
+      <c r="E4" s="7"/>
+      <c r="F4" s="7"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="7" t="s">
+        <v>10</v>
+      </c>
+      <c r="B5" s="7"/>
+      <c r="C5" s="7"/>
+      <c r="D5" s="7"/>
+      <c r="E5" s="7"/>
+      <c r="F5" s="7"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="7" t="s">
+        <v>11</v>
+      </c>
+      <c r="B6" s="8"/>
+      <c r="C6" s="8"/>
+      <c r="D6" s="8"/>
+      <c r="E6" s="8"/>
+      <c r="F6" s="7"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A1:F1"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>

</xml_diff>

<commit_message>
✨ feat((111 - 152)):
</commit_message>
<xml_diff>
--- a/config/cfg_template.xlsx
+++ b/config/cfg_template.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="3" lowestEdited="5" rupBuild="9302"/>
   <workbookPr/>
   <bookViews>
-    <workbookView windowWidth="25600" windowHeight="9560" firstSheet="15" activeTab="16"/>
+    <workbookView windowWidth="25600" windowHeight="8240" firstSheet="20" activeTab="20"/>
   </bookViews>
   <sheets>
     <sheet name="JSBG_7_PH-(表层样PH分级)" sheetId="1" r:id="rId1"/>
@@ -23,14 +23,54 @@
     <sheet name="JSBG_49_AMO-(表层样AMO分级)" sheetId="15" r:id="rId14"/>
     <sheet name="JSBG_53_GZCHD-(表层样GZCHD分级)" sheetId="16" r:id="rId15"/>
     <sheet name="TRSX_111_PH-(利用类型pH面积分级)" sheetId="3" r:id="rId16"/>
-    <sheet name="TRSX_135_OM-(利用类型OM面积分级)" sheetId="17" r:id="rId17"/>
+    <sheet name="TRSX_112_PH-(街道PH面积分级)" sheetId="18" r:id="rId17"/>
+    <sheet name="TRSX_113_PH-(土类PH面积分级)" sheetId="19" r:id="rId18"/>
+    <sheet name="TRSX_114_CEC-(利用类型ECE面积分级)" sheetId="20" r:id="rId19"/>
+    <sheet name="TRSX_115_CEC-(街道ECE面积分级)" sheetId="21" r:id="rId20"/>
+    <sheet name="TRSX_116_CEC-(土类ECE面积分级)" sheetId="22" r:id="rId21"/>
+    <sheet name="TRSX_117_TRRZPJZ-(利用类型容重面积分级)" sheetId="23" r:id="rId22"/>
+    <sheet name="TRSX_118_TRRZPJZ-(街道容重面积分级)" sheetId="24" r:id="rId23"/>
+    <sheet name="TRSX_119_TRRZPJZ-(土类容重面积分级)" sheetId="25" r:id="rId24"/>
+    <sheet name="TRSX_120_GZCHD" sheetId="26" r:id="rId25"/>
+    <sheet name="TRSX_121_GZCHD" sheetId="27" r:id="rId26"/>
+    <sheet name="TRSX_122_GZCHD" sheetId="28" r:id="rId27"/>
+    <sheet name="TRSX_123_TRZD" sheetId="29" r:id="rId28"/>
+    <sheet name="TRSX_124_TRZD" sheetId="30" r:id="rId29"/>
+    <sheet name="TRSX_125_TRZD" sheetId="31" r:id="rId30"/>
+    <sheet name="TRSX_126_TRSL" sheetId="32" r:id="rId31"/>
+    <sheet name="TRSX_127_TRSL" sheetId="33" r:id="rId32"/>
+    <sheet name="TRSX_128_TRSL" sheetId="34" r:id="rId33"/>
+    <sheet name="TRSX_129_TRFSL" sheetId="35" r:id="rId34"/>
+    <sheet name="TRSX_130_TRFSL" sheetId="36" r:id="rId35"/>
+    <sheet name="TRSX_131_TRFSL" sheetId="37" r:id="rId36"/>
+    <sheet name="TRSX_132_TRNL" sheetId="38" r:id="rId37"/>
+    <sheet name="TRSX_133_TRNL" sheetId="39" r:id="rId38"/>
+    <sheet name="TRSX_134_TRNL" sheetId="40" r:id="rId39"/>
+    <sheet name="TRSX_135_OM-(利用类型OM面积分级)" sheetId="17" r:id="rId40"/>
+    <sheet name="TRSX_136_OM" sheetId="41" r:id="rId41"/>
+    <sheet name="TRSX_137_OM" sheetId="42" r:id="rId42"/>
+    <sheet name="TRSX_138_TN" sheetId="43" r:id="rId43"/>
+    <sheet name="TRSX_139_TN" sheetId="44" r:id="rId44"/>
+    <sheet name="TRSX_140_TN" sheetId="45" r:id="rId45"/>
+    <sheet name="TRSX_141_TP" sheetId="46" r:id="rId46"/>
+    <sheet name="TRSX_142_TP" sheetId="47" r:id="rId47"/>
+    <sheet name="TRSX_143_TP" sheetId="48" r:id="rId48"/>
+    <sheet name="TRSX_144_TK" sheetId="49" r:id="rId49"/>
+    <sheet name="TRSX_145_TK" sheetId="50" r:id="rId50"/>
+    <sheet name="TRSX_146_TK" sheetId="51" r:id="rId51"/>
+    <sheet name="TRSX_147_AP" sheetId="52" r:id="rId52"/>
+    <sheet name="TRSX_148_AP" sheetId="53" r:id="rId53"/>
+    <sheet name="TRSX_149_AP" sheetId="54" r:id="rId54"/>
+    <sheet name="TRSX_150_AK" sheetId="55" r:id="rId55"/>
+    <sheet name="TRSX_151_AK" sheetId="56" r:id="rId56"/>
+    <sheet name="TRSX_152_AK" sheetId="57" r:id="rId57"/>
   </sheets>
   <calcPr calcId="144525"/>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="266" uniqueCount="114">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="727" uniqueCount="191">
   <si>
     <t>A1</t>
   </si>
@@ -356,6 +396,169 @@
     <t>合计</t>
   </si>
   <si>
+    <t>XX县各乡镇（街道）土壤pH分级面积统计表</t>
+  </si>
+  <si>
+    <t>乡镇/街道</t>
+  </si>
+  <si>
+    <t>XX县不同土类土壤pH分级面积统计表</t>
+  </si>
+  <si>
+    <t>土类</t>
+  </si>
+  <si>
+    <t>XX县土地利用类型土壤阳离子交换量分级面积统计表</t>
+  </si>
+  <si>
+    <t>&gt;30.0</t>
+  </si>
+  <si>
+    <t>20.0-30.0</t>
+  </si>
+  <si>
+    <t>10.0-20.0</t>
+  </si>
+  <si>
+    <t>5.0-10.0</t>
+  </si>
+  <si>
+    <t>≤5.0</t>
+  </si>
+  <si>
+    <t>XX县各乡镇（街道）土壤阳离子交换量分级面积统计表</t>
+  </si>
+  <si>
+    <t>XX县不同土类土壤阳离子交换量分级面积统计表</t>
+  </si>
+  <si>
+    <t>XX县土地利用类型土壤容重分级面积统计表</t>
+  </si>
+  <si>
+    <t>1.00-1.20</t>
+  </si>
+  <si>
+    <t>1.20-1.30,
+0.90-1.00</t>
+  </si>
+  <si>
+    <t>1.30-1.40</t>
+  </si>
+  <si>
+    <t>1.40-1.50</t>
+  </si>
+  <si>
+    <t>&gt;1.50，≤0.90</t>
+  </si>
+  <si>
+    <t>XX县各乡镇（街道）土壤容重分级面积统计表</t>
+  </si>
+  <si>
+    <t>XX县不同土类土壤容重分级面积统计表</t>
+  </si>
+  <si>
+    <t>XX县土地利用类型土壤耕作层厚度分级面积统计表</t>
+  </si>
+  <si>
+    <t>&gt;20.0</t>
+  </si>
+  <si>
+    <t>16.0-20.0</t>
+  </si>
+  <si>
+    <t>12.0-16.0</t>
+  </si>
+  <si>
+    <t>8.0-12.0</t>
+  </si>
+  <si>
+    <t>≤8.0</t>
+  </si>
+  <si>
+    <t>XX县各乡镇（街道）土壤耕作层厚度分级面积统计表</t>
+  </si>
+  <si>
+    <t>XX县不同土类土壤耕作层厚度分级面积统计表</t>
+  </si>
+  <si>
+    <t>XX县土地利用类型土壤质地面积统计表</t>
+  </si>
+  <si>
+    <t>砂土</t>
+  </si>
+  <si>
+    <t>砂壤</t>
+  </si>
+  <si>
+    <t>轻壤</t>
+  </si>
+  <si>
+    <t>中壤</t>
+  </si>
+  <si>
+    <t>重壤</t>
+  </si>
+  <si>
+    <t>黏土</t>
+  </si>
+  <si>
+    <t>XX县乡镇（街道）土壤质地面积统计表</t>
+  </si>
+  <si>
+    <t>XX县不同土类土壤质地面积统计表</t>
+  </si>
+  <si>
+    <t>XX县土地利用类型土壤砂粒含量分级面积统计表</t>
+  </si>
+  <si>
+    <t>30%~35%</t>
+  </si>
+  <si>
+    <t>35%~40%</t>
+  </si>
+  <si>
+    <t>40%~45%</t>
+  </si>
+  <si>
+    <t>45%~50%</t>
+  </si>
+  <si>
+    <t>&gt;50%</t>
+  </si>
+  <si>
+    <t>XX县各乡镇（街道）土壤砂粒含量分级面积统计表</t>
+  </si>
+  <si>
+    <t>XX县不同土类土壤砂粒含量分级面积统计表</t>
+  </si>
+  <si>
+    <t>XX县土地利用类型土壤粉砂粒含量分级面积统计表</t>
+  </si>
+  <si>
+    <t>20%~25%</t>
+  </si>
+  <si>
+    <t>25%~30%</t>
+  </si>
+  <si>
+    <t>&gt;35%</t>
+  </si>
+  <si>
+    <t>XX县各乡镇（街道）土壤粉砂粒含量分级面积统计表</t>
+  </si>
+  <si>
+    <t>XX县不同土类土壤粉砂粒含量分级面积统计表</t>
+  </si>
+  <si>
+    <t>XX县土地利用类型土壤黏粒含量分级面积统计表</t>
+  </si>
+  <si>
+    <t>XX县各乡镇（街道）土壤黏粒含量分级面积统计表</t>
+  </si>
+  <si>
+    <t>XX县土类土壤黏粒含量分级面积统计表</t>
+  </si>
+  <si>
     <t>XX县土地利用类型土壤有机质含量分级面积统计表</t>
   </si>
   <si>
@@ -372,6 +575,75 @@
   </si>
   <si>
     <t>≤10.0</t>
+  </si>
+  <si>
+    <t>XX县各乡镇（街道）土壤有机质含量分级面积统计表</t>
+  </si>
+  <si>
+    <t>XX县不同土类土壤有机质含量分级面积统计表</t>
+  </si>
+  <si>
+    <t>XX县土地利用类型土壤全氮含量分级面积统计表</t>
+  </si>
+  <si>
+    <t>&gt;2.0</t>
+  </si>
+  <si>
+    <t>XX县各乡镇（街道）土壤全氮含量分级面积统计表</t>
+  </si>
+  <si>
+    <t>XX县不同土类土壤全氮含量分级面积统计表</t>
+  </si>
+  <si>
+    <t>XX县土地利用类型土壤全磷含量分级面积统计表</t>
+  </si>
+  <si>
+    <t>XX县各乡镇（街道）土壤全磷含量分级面积统计表</t>
+  </si>
+  <si>
+    <t>XX县不同土类土壤全磷含量分级面积统计表</t>
+  </si>
+  <si>
+    <t>XX县土地利用类型土壤全钾含量分级面积统计表</t>
+  </si>
+  <si>
+    <t>20.0~25.0</t>
+  </si>
+  <si>
+    <t>15.0~20.0</t>
+  </si>
+  <si>
+    <t>10.0~15.0</t>
+  </si>
+  <si>
+    <t>XX县各乡镇（街道）土壤全钾含量分级面积统计表</t>
+  </si>
+  <si>
+    <t>XX县不同土类土壤全钾含量分级面积统计表</t>
+  </si>
+  <si>
+    <t>XX县土地利用类型土壤有效磷含量分级面积统计表</t>
+  </si>
+  <si>
+    <t>25.0~35.0</t>
+  </si>
+  <si>
+    <t>15.0~25.0</t>
+  </si>
+  <si>
+    <t>XX县各乡镇（街道）土壤有效磷含量分级面积统计表</t>
+  </si>
+  <si>
+    <t>XX县不同土类土壤有效磷含量分级面积统计表</t>
+  </si>
+  <si>
+    <t>XX县土地利用类型土壤速效钾含量分级面积统计表</t>
+  </si>
+  <si>
+    <t>XX县乡镇（街道）土壤速效钾含量分级面积统计表</t>
+  </si>
+  <si>
+    <t>XX县不同土类土壤速效钾含量分级面积统计表</t>
   </si>
 </sst>
 </file>
@@ -556,7 +828,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="34">
+  <fills count="35">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -566,6 +838,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor rgb="FFF1F1F1"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFE7E6E6"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -929,7 +1207,7 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="0" fillId="4" borderId="4" applyNumberFormat="0" applyFont="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
@@ -953,16 +1231,16 @@
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="12" fillId="4" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="12" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="13" fillId="5" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="13" fillId="6" borderId="8" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="14" fillId="5" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="14" fillId="6" borderId="7" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="15" fillId="6" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="15" fillId="7" borderId="9" applyNumberFormat="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="16" fillId="0" borderId="10" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
@@ -971,89 +1249,89 @@
     <xf numFmtId="0" fontId="17" fillId="0" borderId="11" applyNumberFormat="0" applyFill="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="18" fillId="7" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="18" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="19" fillId="8" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="19" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="9" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="20" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="10" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="22" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="11" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="12" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="13" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="14" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="15" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="16" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="17" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="18" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="19" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="20" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="21" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="22" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="23" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="24" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="25" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="26" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="27" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="28" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="29" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="21" fillId="30" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="22" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="21" fillId="31" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="22" fillId="32" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="21" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+    <xf numFmtId="0" fontId="22" fillId="33" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
       <alignment vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="21" fillId="34" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0">
+      <alignment vertical="center"/>
+    </xf>
   </cellStyleXfs>
-  <cellXfs count="14">
+  <cellXfs count="16">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0">
       <alignment vertical="center"/>
     </xf>
@@ -1071,6 +1349,12 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1">
       <alignment vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="2" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1635,17 +1919,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>1</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1665,7 +1949,7 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="8" t="s">
+      <c r="A3" s="10" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1677,43 +1961,43 @@
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="13" t="str">
+      <c r="B4" s="15" t="str">
         <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
         <v>B4</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="13" t="str">
+      <c r="B5" s="15" t="str">
         <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
         <v>B5</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="13" t="str">
+      <c r="B6" s="15" t="str">
         <f>SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
         <v>B6</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1746,7 +2030,7 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>59</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1766,54 +2050,54 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>60</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="11" t="s">
         <v>61</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="11" t="s">
         <v>62</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="11" t="s">
         <v>63</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="11" t="s">
         <v>64</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1846,7 +2130,7 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>66</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1866,54 +2150,54 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>67</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="11" t="s">
         <v>68</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="11" t="s">
         <v>69</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="11" t="s">
         <v>70</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="11" t="s">
         <v>71</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="9"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -1946,7 +2230,7 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>73</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1966,54 +2250,54 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>74</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="11" t="s">
         <v>75</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="11" t="s">
         <v>78</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2046,7 +2330,7 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>80</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2066,54 +2350,54 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="11" t="s">
         <v>76</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="11" t="s">
         <v>77</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="11" t="s">
         <v>81</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="11" t="s">
         <v>82</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="9"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="B6" s="11"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2146,7 +2430,7 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>84</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2166,54 +2450,54 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>85</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="11" t="s">
         <v>86</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="11" t="s">
         <v>87</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="11" t="s">
         <v>88</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="11" t="s">
         <v>89</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2246,7 +2530,7 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>91</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2266,54 +2550,54 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="11" t="s">
         <v>92</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="11" t="s">
         <v>93</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="11" t="s">
         <v>94</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="11" t="s">
         <v>95</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -2330,7 +2614,7 @@
   <dimension ref="A1:F8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="M19" sqref="M19"/>
+      <selection activeCell="K5" sqref="K5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="7" outlineLevelCol="5"/>
@@ -2351,7 +2635,7 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="6" t="s">
+      <c r="A2" s="8" t="s">
         <v>97</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2371,7 +2655,7 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="7"/>
+      <c r="A3" s="9"/>
       <c r="B3" s="2" t="s">
         <v>98</v>
       </c>
@@ -2451,13 +2735,13 @@
 <file path=xl/worksheets/sheet17.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
   <sheetPr/>
-  <dimension ref="A1:F8"/>
+  <dimension ref="A1:F3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="J21" sqref="J21"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H3" sqref="H3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="7" outlineLevelCol="5"/>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
   <sheetData>
     <row r="1" spans="1:6">
       <c r="A1" s="1" t="s">
@@ -2471,7 +2755,7 @@
     </row>
     <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
-        <v>97</v>
+        <v>109</v>
       </c>
       <c r="B2" s="2" t="s">
         <v>2</v>
@@ -2492,70 +2776,165 @@
     <row r="3" spans="1:6">
       <c r="A3" s="2"/>
       <c r="B3" s="2" t="s">
-        <v>109</v>
+        <v>98</v>
       </c>
       <c r="C3" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>100</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet18.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
         <v>110</v>
       </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>99</v>
+      </c>
       <c r="D3" s="2" t="s">
-        <v>111</v>
+        <v>100</v>
       </c>
       <c r="E3" s="2" t="s">
+        <v>101</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>102</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet19.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I19" sqref="I19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="13.6153846153846" customWidth="1"/>
+    <col min="2" max="2" width="7.07692307692308" customWidth="1"/>
+    <col min="3" max="4" width="10.3846153846154" customWidth="1"/>
+    <col min="5" max="5" width="9.23076923076923" customWidth="1"/>
+    <col min="6" max="6" width="5.92307692307692" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
         <v>112</v>
       </c>
-      <c r="F3" s="2" t="s">
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="6" t="s">
         <v>113</v>
       </c>
-    </row>
-    <row r="4" spans="1:6">
-      <c r="A4" s="3" t="s">
-        <v>103</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
-      <c r="E4" s="4"/>
-      <c r="F4" s="5"/>
-    </row>
-    <row r="5" spans="1:6">
-      <c r="A5" s="3" t="s">
-        <v>104</v>
-      </c>
-      <c r="B5" s="4"/>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
-      <c r="E5" s="4"/>
-      <c r="F5" s="5"/>
-    </row>
-    <row r="6" spans="1:6">
-      <c r="A6" s="3" t="s">
-        <v>105</v>
-      </c>
-      <c r="B6" s="4"/>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
-      <c r="E6" s="4"/>
-      <c r="F6" s="5"/>
-    </row>
-    <row r="7" spans="1:6">
-      <c r="A7" s="3" t="s">
-        <v>106</v>
-      </c>
-      <c r="B7" s="4"/>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
-      <c r="E7" s="4"/>
-      <c r="F7" s="5"/>
-    </row>
-    <row r="8" spans="1:6">
-      <c r="A8" s="3" t="s">
-        <v>107</v>
-      </c>
-      <c r="B8" s="5"/>
-      <c r="C8" s="5"/>
-      <c r="D8" s="5"/>
-      <c r="E8" s="5"/>
-      <c r="F8" s="5"/>
+      <c r="C3" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>117</v>
+      </c>
     </row>
   </sheetData>
   <mergeCells count="2">
@@ -2585,17 +2964,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:6">
-      <c r="A1" s="11" t="s">
+      <c r="A1" s="13" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="11"/>
-      <c r="C1" s="11"/>
-      <c r="D1" s="11"/>
-      <c r="E1" s="11"/>
-      <c r="F1" s="11"/>
+      <c r="B1" s="13"/>
+      <c r="C1" s="13"/>
+      <c r="D1" s="13"/>
+      <c r="E1" s="13"/>
+      <c r="F1" s="13"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>12</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2615,7 +2994,7 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="12" t="s">
+      <c r="A3" s="14" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -2627,47 +3006,767 @@
       <c r="F3" s="2"/>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="12" t="s">
+      <c r="A4" s="14" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="13" t="str">
+      <c r="B4" s="15" t="str">
         <f t="shared" ref="B4:B6" si="0">SUBSTITUTE(ADDRESS(ROW(),COLUMN()),"$","")</f>
         <v>B4</v>
       </c>
-      <c r="C4" s="13"/>
-      <c r="D4" s="13"/>
-      <c r="E4" s="13"/>
-      <c r="F4" s="13"/>
+      <c r="C4" s="15"/>
+      <c r="D4" s="15"/>
+      <c r="E4" s="15"/>
+      <c r="F4" s="15"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="12" t="s">
+      <c r="A5" s="14" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="13" t="str">
+      <c r="B5" s="15" t="str">
         <f t="shared" si="0"/>
         <v>B5</v>
       </c>
-      <c r="C5" s="13"/>
-      <c r="D5" s="13"/>
-      <c r="E5" s="13"/>
-      <c r="F5" s="13"/>
+      <c r="C5" s="15"/>
+      <c r="D5" s="15"/>
+      <c r="E5" s="15"/>
+      <c r="F5" s="15"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="12" t="s">
+      <c r="A6" s="14" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="13" t="str">
+      <c r="B6" s="15" t="str">
         <f t="shared" si="0"/>
         <v>B6</v>
       </c>
-      <c r="C6" s="13"/>
-      <c r="D6" s="13"/>
-      <c r="E6" s="13"/>
-      <c r="F6" s="13"/>
+      <c r="C6" s="15"/>
+      <c r="D6" s="15"/>
+      <c r="E6" s="15"/>
+      <c r="F6" s="15"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet20.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>118</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet21.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G16" sqref="G16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>119</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="6" t="s">
+        <v>113</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>114</v>
+      </c>
+      <c r="D3" s="6" t="s">
+        <v>115</v>
+      </c>
+      <c r="E3" s="6" t="s">
+        <v>116</v>
+      </c>
+      <c r="F3" s="6" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet22.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I15" sqref="I15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <cols>
+    <col min="1" max="1" width="13.6153846153846" customWidth="1"/>
+    <col min="2" max="2" width="10.3846153846154" customWidth="1"/>
+    <col min="3" max="3" width="5.57692307692308" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" ht="61" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet23.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>126</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" ht="61" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet24.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="J15" sqref="J15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>127</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" ht="61" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="6" t="s">
+        <v>121</v>
+      </c>
+      <c r="C3" s="7" t="s">
+        <v>122</v>
+      </c>
+      <c r="D3" s="7" t="s">
+        <v>123</v>
+      </c>
+      <c r="E3" s="7" t="s">
+        <v>124</v>
+      </c>
+      <c r="F3" s="7" t="s">
+        <v>125</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet25.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>128</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet26.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>134</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet27.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>135</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>129</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>130</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>131</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>132</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>133</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet28.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A2:G8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="E17" sqref="E17"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="7" outlineLevelCol="6"/>
+  <sheetData>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>136</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="4" spans="1:7">
+      <c r="A4" s="4" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="4"/>
+      <c r="G4" s="5"/>
+    </row>
+    <row r="5" spans="1:7">
+      <c r="A5" s="4" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="4"/>
+      <c r="G5" s="5"/>
+    </row>
+    <row r="6" spans="1:7">
+      <c r="A6" s="4" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="4"/>
+      <c r="G6" s="5"/>
+    </row>
+    <row r="7" spans="1:7">
+      <c r="A7" s="4" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="4"/>
+      <c r="G7" s="5"/>
+    </row>
+    <row r="8" spans="1:7">
+      <c r="A8" s="4" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="4"/>
+      <c r="C8" s="4"/>
+      <c r="D8" s="4"/>
+      <c r="E8" s="4"/>
+      <c r="F8" s="4"/>
+      <c r="G8" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet29.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A2:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A2" sqref="A2:G3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="6"/>
+  <sheetData>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>143</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:G2"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -2696,7 +3795,7 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>14</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2716,58 +3815,691 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>15</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="11" t="s">
         <v>16</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="11" t="s">
         <v>17</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="11" t="s">
         <v>18</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="11" t="s">
         <v>19</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet30.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A2:G3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A4" sqref="A4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="6"/>
+  <sheetData>
+    <row r="2" spans="1:7">
+      <c r="A2" s="1" t="s">
+        <v>144</v>
+      </c>
+      <c r="B2" s="1"/>
+      <c r="C2" s="1"/>
+      <c r="D2" s="1"/>
+      <c r="E2" s="1"/>
+      <c r="F2" s="1"/>
+      <c r="G2" s="1"/>
+    </row>
+    <row r="3" spans="1:7">
+      <c r="A3" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B3" s="2" t="s">
+        <v>137</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>138</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>139</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>140</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>141</v>
+      </c>
+      <c r="G3" s="2" t="s">
+        <v>142</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="1">
+    <mergeCell ref="A2:G2"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet31.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>145</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet32.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>151</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet33.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="J16" sqref="J16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>152</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>147</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>148</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>149</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>150</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet34.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>153</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet35.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>157</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet36.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>158</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet37.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>159</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet38.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:E3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>160</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet39.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:E3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H4" sqref="H4"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="4"/>
+  <sheetData>
+    <row r="1" spans="1:5">
+      <c r="A1" s="1" t="s">
+        <v>161</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+    </row>
+    <row r="2" spans="1:5">
+      <c r="A2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:5">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>154</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>155</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>146</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>156</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:E1"/>
+    <mergeCell ref="A2:A3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -2796,7 +4528,7 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>21</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2816,58 +4548,798 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>22</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="11" t="s">
         <v>25</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="11" t="s">
         <v>26</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet40.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F8"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G9" sqref="G9"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="7" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>162</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="4" spans="1:6">
+      <c r="A4" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="4"/>
+      <c r="D4" s="4"/>
+      <c r="E4" s="4"/>
+      <c r="F4" s="5"/>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="4"/>
+      <c r="D5" s="4"/>
+      <c r="E5" s="4"/>
+      <c r="F5" s="5"/>
+    </row>
+    <row r="6" spans="1:6">
+      <c r="A6" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="B6" s="4"/>
+      <c r="C6" s="4"/>
+      <c r="D6" s="4"/>
+      <c r="E6" s="4"/>
+      <c r="F6" s="5"/>
+    </row>
+    <row r="7" spans="1:6">
+      <c r="A7" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="B7" s="4"/>
+      <c r="C7" s="4"/>
+      <c r="D7" s="4"/>
+      <c r="E7" s="4"/>
+      <c r="F7" s="5"/>
+    </row>
+    <row r="8" spans="1:6">
+      <c r="A8" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="B8" s="5"/>
+      <c r="C8" s="5"/>
+      <c r="D8" s="5"/>
+      <c r="E8" s="5"/>
+      <c r="F8" s="5"/>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet41.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>168</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet42.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="K15" sqref="K15"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>169</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>163</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>164</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>165</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>166</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet43.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>170</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet44.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>172</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet45.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>173</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>171</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>19</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet46.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>174</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet47.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>175</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet48.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>176</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>22</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>23</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>24</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>26</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet49.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>177</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -2896,7 +5368,7 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>28</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -2916,58 +5388,610 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="11" t="s">
         <v>30</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="11" t="s">
         <v>31</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="11" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
     <mergeCell ref="A1:F1"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet50.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>181</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet51.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>182</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>29</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>178</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>179</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet52.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>183</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet53.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>186</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet54.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>187</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>36</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>184</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>185</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>180</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>167</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet55.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>188</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>97</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet56.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A1" sqref="A1:F3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>189</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>109</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
+  </mergeCells>
+  <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
+  <headerFooter/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet57.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:etc="http://www.wps.cn/officeDocument/2017/etCustomData">
+  <sheetPr/>
+  <dimension ref="A1:F3"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G10" sqref="G10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultColWidth="9.23076923076923" defaultRowHeight="16.8" outlineLevelRow="2" outlineLevelCol="5"/>
+  <sheetData>
+    <row r="1" spans="1:6">
+      <c r="A1" s="1" t="s">
+        <v>190</v>
+      </c>
+      <c r="B1" s="1"/>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+    </row>
+    <row r="2" spans="1:6">
+      <c r="A2" s="2" t="s">
+        <v>111</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>2</v>
+      </c>
+      <c r="C2" s="2" t="s">
+        <v>3</v>
+      </c>
+      <c r="D2" s="2" t="s">
+        <v>4</v>
+      </c>
+      <c r="E2" s="2" t="s">
+        <v>5</v>
+      </c>
+      <c r="F2" s="2" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="3" spans="1:6">
+      <c r="A3" s="2"/>
+      <c r="B3" s="2" t="s">
+        <v>41</v>
+      </c>
+      <c r="C3" s="2" t="s">
+        <v>42</v>
+      </c>
+      <c r="D3" s="2" t="s">
+        <v>43</v>
+      </c>
+      <c r="E3" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="F3" s="2" t="s">
+        <v>45</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="A1:F1"/>
+    <mergeCell ref="A2:A3"/>
   </mergeCells>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter/>
@@ -2996,7 +6020,7 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>35</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -3016,54 +6040,54 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>36</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="11" t="s">
         <v>37</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="11" t="s">
         <v>38</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="11" t="s">
         <v>32</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="11" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3096,7 +6120,7 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>40</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -3116,7 +6140,7 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -3136,34 +6160,34 @@
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3196,7 +6220,7 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>47</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -3216,54 +6240,54 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>48</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="11" t="s">
         <v>49</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="11" t="s">
         <v>50</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="11" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="10"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12"/>
     </row>
   </sheetData>
   <mergeCells count="1">
@@ -3296,7 +6320,7 @@
       <c r="F1" s="1"/>
     </row>
     <row r="2" spans="1:6">
-      <c r="A2" s="8" t="s">
+      <c r="A2" s="10" t="s">
         <v>53</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -3316,54 +6340,54 @@
       </c>
     </row>
     <row r="3" spans="1:6">
-      <c r="A3" s="9" t="s">
+      <c r="A3" s="11" t="s">
         <v>7</v>
       </c>
-      <c r="B3" s="9" t="s">
+      <c r="B3" s="11" t="s">
         <v>54</v>
       </c>
-      <c r="C3" s="9" t="s">
+      <c r="C3" s="11" t="s">
         <v>51</v>
       </c>
-      <c r="D3" s="9" t="s">
+      <c r="D3" s="11" t="s">
         <v>55</v>
       </c>
-      <c r="E3" s="9" t="s">
+      <c r="E3" s="11" t="s">
         <v>56</v>
       </c>
-      <c r="F3" s="9" t="s">
+      <c r="F3" s="11" t="s">
         <v>57</v>
       </c>
     </row>
     <row r="4" spans="1:6">
-      <c r="A4" s="9" t="s">
+      <c r="A4" s="11" t="s">
         <v>9</v>
       </c>
-      <c r="B4" s="9"/>
-      <c r="C4" s="9"/>
-      <c r="D4" s="9"/>
-      <c r="E4" s="9"/>
-      <c r="F4" s="9"/>
+      <c r="B4" s="11"/>
+      <c r="C4" s="11"/>
+      <c r="D4" s="11"/>
+      <c r="E4" s="11"/>
+      <c r="F4" s="11"/>
     </row>
     <row r="5" spans="1:6">
-      <c r="A5" s="9" t="s">
+      <c r="A5" s="11" t="s">
         <v>10</v>
       </c>
-      <c r="B5" s="9"/>
-      <c r="C5" s="9"/>
-      <c r="D5" s="9"/>
-      <c r="E5" s="9"/>
-      <c r="F5" s="9"/>
+      <c r="B5" s="11"/>
+      <c r="C5" s="11"/>
+      <c r="D5" s="11"/>
+      <c r="E5" s="11"/>
+      <c r="F5" s="11"/>
     </row>
     <row r="6" spans="1:6">
-      <c r="A6" s="9" t="s">
+      <c r="A6" s="11" t="s">
         <v>11</v>
       </c>
-      <c r="B6" s="10"/>
-      <c r="C6" s="10"/>
-      <c r="D6" s="10"/>
-      <c r="E6" s="10"/>
-      <c r="F6" s="9"/>
+      <c r="B6" s="12"/>
+      <c r="C6" s="12"/>
+      <c r="D6" s="12"/>
+      <c r="E6" s="12"/>
+      <c r="F6" s="11"/>
     </row>
   </sheetData>
   <mergeCells count="1">

</xml_diff>